<commit_message>
get task 1 running
</commit_message>
<xml_diff>
--- a/version01/1_task/CAMELlocal/config/languageFile.xlsx
+++ b/version01/1_task/CAMELlocal/config/languageFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fenn\Nextcloud\Artikel Cognitive Affective Maps Tools\CAM tools\CAMtools_CAMEL\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3BDC19-247E-4E80-8730-3BF5B7CFDD70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35ACCA7-EEB7-4EB5-9480-05EA20B98ADF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,9 +532,6 @@
     <t>set concept to</t>
   </si>
   <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>nd_02</t>
   </si>
   <si>
@@ -838,12 +835,6 @@
     <t>Declarar que concepto es</t>
   </si>
   <si>
-    <t>Kommentar</t>
-  </si>
-  <si>
-    <t>Comentario</t>
-  </si>
-  <si>
     <t>Art und Stärke der Verbindung</t>
   </si>
   <si>
@@ -1450,9 +1441,6 @@
     <t>Définir le concept comme</t>
   </si>
   <si>
-    <t>Commentaire</t>
-  </si>
-  <si>
     <t>Supprimer le concept</t>
   </si>
   <si>
@@ -1732,9 +1720,6 @@
     <t>设置概念为</t>
   </si>
   <si>
-    <t>注释</t>
-  </si>
-  <si>
     <t>删除概念</t>
   </si>
   <si>
@@ -1889,6 +1874,21 @@
   </si>
   <si>
     <t xml:space="preserve"> contain less than 3 letters.</t>
+  </si>
+  <si>
+    <t>Comment:</t>
+  </si>
+  <si>
+    <t>Kommentar:</t>
+  </si>
+  <si>
+    <t>Commentaire:</t>
+  </si>
+  <si>
+    <t>Comentario:</t>
+  </si>
+  <si>
+    <t>注释:</t>
   </si>
 </sst>
 </file>
@@ -2275,8 +2275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2308,7 +2308,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="H1" t="s">
         <v>56</v>
@@ -2319,25 +2319,25 @@
     </row>
     <row r="2" spans="1:9" ht="105">
       <c r="A2" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -2351,16 +2351,16 @@
         <v>73</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="120">
@@ -2374,39 +2374,39 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>361</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>113</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60">
@@ -2420,16 +2420,16 @@
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>429</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>117</v>
-      </c>
       <c r="G6" s="2" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -2443,16 +2443,16 @@
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2466,16 +2466,16 @@
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2489,16 +2489,16 @@
         <v>19</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -2512,16 +2512,16 @@
         <v>20</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="60">
@@ -2535,16 +2535,16 @@
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>367</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>127</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30">
@@ -2558,16 +2558,16 @@
         <v>22</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="30">
@@ -2578,65 +2578,65 @@
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30">
       <c r="A14" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="60">
       <c r="A15" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="30">
@@ -2650,16 +2650,16 @@
         <v>24</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="45">
@@ -2673,16 +2673,16 @@
         <v>28</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="45">
@@ -2696,16 +2696,16 @@
         <v>29</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="105">
@@ -2716,19 +2716,19 @@
         <v>2</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30">
@@ -2742,16 +2742,16 @@
         <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="60">
@@ -2765,16 +2765,16 @@
         <v>40</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>375</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>140</v>
-      </c>
       <c r="G21" s="2" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="105">
@@ -2788,16 +2788,16 @@
         <v>41</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="75">
@@ -2808,19 +2808,19 @@
         <v>2</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>144</v>
-      </c>
       <c r="G23" s="2" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="30">
@@ -2834,16 +2834,16 @@
         <v>39</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>431</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="60">
@@ -2857,16 +2857,16 @@
         <v>42</v>
       </c>
       <c r="D25" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="F25" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>148</v>
-      </c>
       <c r="G25" s="2" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="45">
@@ -2880,16 +2880,16 @@
         <v>43</v>
       </c>
       <c r="D26" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>150</v>
-      </c>
       <c r="G26" s="2" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="105">
@@ -2900,19 +2900,19 @@
         <v>2</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>152</v>
-      </c>
       <c r="G27" s="2" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="30">
@@ -2926,16 +2926,16 @@
         <v>49</v>
       </c>
       <c r="D28" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>432</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="G28" s="2" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="120">
@@ -2949,39 +2949,39 @@
         <v>50</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="75">
       <c r="A30" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
     </row>
     <row r="31" spans="1:7">
@@ -2995,16 +2995,16 @@
         <v>51</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="30">
@@ -3018,16 +3018,16 @@
         <v>52</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="60">
@@ -3041,16 +3041,16 @@
         <v>53</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="45">
@@ -3064,16 +3064,16 @@
         <v>58</v>
       </c>
       <c r="D34" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>434</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>169</v>
-      </c>
       <c r="G34" s="2" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="60">
@@ -3084,19 +3084,19 @@
         <v>2</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="45">
@@ -3107,19 +3107,19 @@
         <v>2</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D36" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>385</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>230</v>
-      </c>
       <c r="G36" s="2" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="60">
@@ -3130,19 +3130,19 @@
         <v>2</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -3156,16 +3156,16 @@
         <v>63</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>387</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>171</v>
-      </c>
       <c r="G38" s="2" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3179,16 +3179,16 @@
         <v>64</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>64</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -3202,16 +3202,16 @@
         <v>65</v>
       </c>
       <c r="D40" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="F40" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>175</v>
-      </c>
       <c r="G40" s="2" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -3228,13 +3228,13 @@
         <v>66</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="30">
@@ -3248,16 +3248,16 @@
         <v>80</v>
       </c>
       <c r="D42" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>178</v>
-      </c>
       <c r="G42" s="2" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="30">
@@ -3271,16 +3271,16 @@
         <v>81</v>
       </c>
       <c r="D43" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="F43" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>180</v>
-      </c>
       <c r="G43" s="2" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="30">
@@ -3294,16 +3294,16 @@
         <v>82</v>
       </c>
       <c r="D44" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="F44" s="3" t="s">
-        <v>182</v>
-      </c>
       <c r="G44" s="2" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -3317,16 +3317,16 @@
         <v>83</v>
       </c>
       <c r="D45" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="G45" s="2" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -3340,21 +3340,21 @@
         <v>86</v>
       </c>
       <c r="D46" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="F46" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="F46" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="G46" s="2" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="30">
       <c r="A47" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>84</v>
@@ -3363,21 +3363,21 @@
         <v>87</v>
       </c>
       <c r="D47" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="F47" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>436</v>
-      </c>
-      <c r="F47" s="3" t="s">
-        <v>188</v>
-      </c>
       <c r="G47" s="2" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="A48" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>84</v>
@@ -3386,1012 +3386,1012 @@
         <v>88</v>
       </c>
       <c r="D48" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>394</v>
-      </c>
-      <c r="F48" s="3" t="s">
-        <v>190</v>
-      </c>
       <c r="G48" s="2" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="A49" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>89</v>
+        <v>537</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>191</v>
+        <v>538</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>395</v>
+        <v>539</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>192</v>
+        <v>540</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>489</v>
+        <v>541</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>84</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="30">
       <c r="A51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>95</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="30">
       <c r="A52" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="30">
       <c r="A53" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="30">
       <c r="A54" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="F54" s="6" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="30">
       <c r="A55" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="30">
       <c r="A56" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>52</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="90">
       <c r="A57" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="30">
       <c r="A58" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="F58" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>401</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>221</v>
-      </c>
       <c r="G58" s="2" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="75">
       <c r="A59" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>250</v>
-      </c>
       <c r="E59" s="3" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="30">
       <c r="A60" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="E60" s="3" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="60">
       <c r="A61" s="1" t="s">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="G61" s="2"/>
     </row>
     <row r="62" spans="1:7" ht="30">
       <c r="A62" s="1" t="s">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="G62" s="2"/>
     </row>
     <row r="63" spans="1:7" ht="60">
       <c r="A63" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="30">
       <c r="A64" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>500</v>
+        <v>495</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="30">
       <c r="A65" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C65" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>244</v>
-      </c>
       <c r="E65" s="2" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>523</v>
+        <v>518</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="75">
       <c r="A66" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
     </row>
     <row r="67" spans="1:7" ht="60">
       <c r="A67" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
     </row>
     <row r="68" spans="1:7" ht="75">
       <c r="A68" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C68" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C68" s="2" t="s">
-        <v>256</v>
-      </c>
       <c r="D68" s="2" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
     </row>
     <row r="69" spans="1:7" ht="30">
       <c r="A69" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>505</v>
+        <v>500</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="45">
       <c r="A70" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>524</v>
+        <v>519</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="105">
       <c r="A71" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>506</v>
+        <v>501</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="150">
       <c r="A72" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>507</v>
+        <v>502</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="60">
       <c r="A73" s="1" t="s">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>529</v>
+        <v>524</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="60">
       <c r="A74" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>288</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B74" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>273</v>
-      </c>
       <c r="D74" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30">
       <c r="A75" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>508</v>
+        <v>503</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="30">
       <c r="A76" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>509</v>
+        <v>504</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="30">
       <c r="A77" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>510</v>
+        <v>505</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="30">
       <c r="A78" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="45">
       <c r="A79" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
     </row>
     <row r="80" spans="1:7" ht="60">
       <c r="A80" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>512</v>
+        <v>507</v>
       </c>
     </row>
     <row r="81" spans="1:7" ht="45">
       <c r="A81" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>515</v>
+        <v>510</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="45">
       <c r="A82" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>513</v>
+        <v>508</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="45">
       <c r="A83" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="G83" s="2" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="45">
       <c r="A84" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B84" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>298</v>
-      </c>
       <c r="D84" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>517</v>
+        <v>512</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="45">
       <c r="A85" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C85" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>306</v>
-      </c>
       <c r="D85" s="2" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G85" s="2" t="s">
-        <v>518</v>
+        <v>513</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="150">
       <c r="A86" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G86" s="2" t="s">
-        <v>519</v>
+        <v>514</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="75">
       <c r="A87" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>525</v>
+        <v>520</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="90">
       <c r="A88" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G88" s="2" t="s">
-        <v>526</v>
+        <v>521</v>
       </c>
     </row>
     <row r="89" spans="1:7">
       <c r="A89" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G89" s="2" t="s">
-        <v>520</v>
+        <v>515</v>
       </c>
     </row>
     <row r="90" spans="1:7">
       <c r="A90" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>521</v>
+        <v>516</v>
       </c>
     </row>
     <row r="91" spans="1:7">
       <c r="A91" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C91" s="2" t="s">
         <v>73</v>
       </c>
       <c r="D91" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="F91" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E91" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>111</v>
-      </c>
       <c r="G91" s="2" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
     </row>
     <row r="92" spans="1:7" ht="30">
       <c r="A92" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="F92" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B92" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>356</v>
-      </c>
-      <c r="D92" s="2" t="s">
-        <v>357</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>430</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>358</v>
-      </c>
       <c r="G92" s="2" t="s">
-        <v>522</v>
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>